<commit_message>
add more chinese-english model name pairs
</commit_message>
<xml_diff>
--- a/device_model translate.xlsx
+++ b/device_model translate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cxy\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3107773-961B-4AB6-970D-0BFA8EEFD5D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F51E2EF-94A1-4F56-A22C-8AC9AF703A73}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7870" yWindow="230" windowWidth="14400" windowHeight="7360" xr2:uid="{8776A762-D09F-4CB4-A5AB-F9C6FD6E8DA9}"/>
+    <workbookView xWindow="4700" yWindow="1130" windowWidth="14400" windowHeight="7360" xr2:uid="{8776A762-D09F-4CB4-A5AB-F9C6FD6E8DA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,138 +31,1176 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="356">
+  <si>
+    <t>乐檬K3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lemeng k3 note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lemeng k3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dazen x7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dazen note3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qiku youth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7295a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>荣耀畅玩4C运动版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>honor 4c sport</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mmang 3s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小米note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mi note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大神F1Plus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dazen f1 plus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黄金斗士Note8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lenovo note8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大神F2全高清版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dazen f2 pro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红米Note2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>红辣椒任性版</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Plus</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>渴望HD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>desire hd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>灵感XL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kiss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>star1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kiss 3n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x315e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>锋尚</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>炫影S+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>大器</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xperia Z1 炫彩版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xperia z1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>samsung b9120</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8720q</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>纽扣</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>飞马</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>星星2号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>star2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zen fone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>button</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lewan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>荣耀7i</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>honor 7i</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超级手机Max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>superphone max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超级手机1 Pro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>superphone 1 pro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mate 7 青春版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mate 7 youth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小辣椒 M3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>倾城L3C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qc l3c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016版 Galaxy A7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016 Galaxy A7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yq601</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>坚果手机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>My 布拉格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>my prague</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小米4C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mi 4c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>红辣椒</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Note</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>apple</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>weike</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>荣耀畅玩平板T1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>honor t1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>红辣椒</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>XM</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三星big foot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>samsung big foot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>领世旗舰3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>samsung g9198</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>畅享5S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enjoy 5s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小鲜2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>xiaoxian 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>锋尚Max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fs max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黄金斗士青春版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lenovo youth</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>红辣椒</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>NX Plus</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chilli m3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chilli 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chilli plus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chilli note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chilli nx plus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chilli xm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chilli</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>倾城L3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qc l3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Axon天机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>axon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>风华3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gn709l</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>么么哒3S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kiss 3s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大器3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>samsung g9092</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小辣椒 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chilli 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天鉴W808</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tj w808</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天鉴W900</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tj w900</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>威武3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>weiwu 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大观铂顿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dag bd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小辣椒 6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chilli 6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黄金斗士S8畅玩版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lenovo s8 pro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小辣椒 X3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chilli x3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jingang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jingang 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>魅蓝Note3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>m1 note 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中兴远航3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zte yh 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>联想VIBE X2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lenovo vibe x2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ltzj</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>coolpad 7290</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天鉴T1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tj t1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>razr v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g719c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小辣椒 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chilli 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chilli 7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>metal 标准版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>metal standard</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zuixiang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>weiwu 3c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lemeng k31</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>乐檬</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>K31</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>火星一号探索版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mars one explore</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>飞马3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zen fone 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>荣耀平板T1-823L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>honor t1-823l</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chilli x4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>moto x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>小辣椒</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> 9</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chilli 9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小辣椒S1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chilli s1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mirror x5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>红辣椒</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Note3</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chilli note3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>土星一号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>saturn one</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>octupos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>红辣椒</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> X1</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chilli x1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t03 fz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>htc a510e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>daq note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016版 Galaxy J7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016 Galaxy J7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>乐檬3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lemeng 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>乐檬X3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lemeng x3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>乐玩2C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lewan 2c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>飞马2 Plus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zen fone 2 plus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>联想S870e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lenovo s870e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>锋尚Air</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fs air</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lenovo tablet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>coolpad 8298</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blf w2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Axon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>天机</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> Max</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>axon max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>superphone max pro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>锋尚mini</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fs mini</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>jupiter one</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>talk 7x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>talk 7x 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>k-touch t619</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chilli 5 pro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小辣椒X5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chilli x5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gimi z3d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>荣耀V8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>honor v8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>axon 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Microsoft YaHei UI"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>联想</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Lucida Console"/>
+        <family val="3"/>
+      </rPr>
+      <t>X2-AP</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lenovo x2-ap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ivvi plus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>original model name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>new model name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设备品类为：平板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>联想黄金斗士S8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>lenovo s8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>黄金斗士A8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>lenovo a8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超级手机1s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>superphone 1s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超级手机1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>superphone 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>超级手机Max Pro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大神F1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dazen f1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大神Note3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大神Note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dazen note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大神X7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大神F2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dazen f2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大神1s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dazen 1s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>redmi note2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红米note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>redmi note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红米1S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>redmi 1s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红米2A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>redmi 2a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红米</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>redmi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红米Note3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>redmi note3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红米3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>redmi 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红米2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>redmi 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红米note增强版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>redmi note pro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>畅享5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>enjoy 5</t>
-  </si>
-  <si>
-    <t>超级手机1s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>superphone 1s</t>
-  </si>
-  <si>
-    <t>超级手机1</t>
-  </si>
-  <si>
-    <t>superphone 1</t>
-  </si>
-  <si>
-    <t>大神F1</t>
-  </si>
-  <si>
-    <t>dazen f1</t>
-  </si>
-  <si>
-    <t>大神Note</t>
-  </si>
-  <si>
-    <t>dazen note</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>大神X7</t>
-  </si>
-  <si>
-    <t>dazen x7</t>
-  </si>
-  <si>
-    <t>大神F2</t>
-  </si>
-  <si>
-    <t>dazen f2</t>
-  </si>
-  <si>
-    <t>大神1s</t>
-  </si>
-  <si>
-    <t>dazen 1s</t>
-  </si>
-  <si>
-    <t>红米Note2</t>
-  </si>
-  <si>
-    <t>redmi note2</t>
-  </si>
-  <si>
-    <t>红米note</t>
-  </si>
-  <si>
-    <t>redmi note</t>
-  </si>
-  <si>
-    <t>红米1S</t>
-  </si>
-  <si>
-    <t>redmi 1s</t>
-  </si>
-  <si>
-    <t>红米2A</t>
-  </si>
-  <si>
-    <t>redmi 2a</t>
-  </si>
-  <si>
-    <t>红米</t>
-  </si>
-  <si>
-    <t>redmi</t>
-  </si>
-  <si>
-    <t>红米Note3</t>
-  </si>
-  <si>
-    <t>redmi note3</t>
-  </si>
-  <si>
-    <t>红米3</t>
-  </si>
-  <si>
-    <t>redmi 3</t>
-  </si>
-  <si>
-    <t>红米2</t>
-  </si>
-  <si>
-    <t>redmi 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>红米note增强版</t>
-  </si>
-  <si>
-    <t>redmi note pro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>荣耀6 Plus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>honor 6 plus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>荣耀3C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>honor 3c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>荣耀6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>honor 6</t>
@@ -170,57 +1208,75 @@
   </si>
   <si>
     <t>荣耀畅玩5X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>honor 5x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>荣耀畅玩4X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>honor 4x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>荣耀畅玩5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>honor 5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>荣耀3C畅玩版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>honor 3c pro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>荣耀U8860</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>honor u8860</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>荣耀畅玩4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>honor 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>荣耀畅玩4C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>honor 4c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>荣耀X2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>honor x2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>荣耀3X畅玩版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>honor 3x pro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>荣耀7</t>
@@ -228,57 +1284,75 @@
   </si>
   <si>
     <t>honor 7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>荣耀4A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>honor 4a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>荣耀6 plus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>荣耀+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>honor +</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>荣耀3X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>honor 3x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>魅蓝metal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>m1 metal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>魅蓝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>m1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>魅蓝2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>m1 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>魅蓝Note 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>m1 note 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>魅蓝NOTE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>m1 note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>note顶配版</t>
@@ -286,69 +1360,83 @@
   </si>
   <si>
     <t>mi note pro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>乐檬K3 Note</t>
-  </si>
-  <si>
-    <t>k3 note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>锋尚Pro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>fs pro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>锋尚2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>fs 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>远航3</t>
-  </si>
-  <si>
-    <t>yh a3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>时尚手机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ss phone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ivvi 小骨Pro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ivvi pro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Z9 mini 精英版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>z9 mini pro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>天鉴W900S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>tj w900s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>小鲜3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>xiaoxian 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>小星星</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>little star</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>2016版 Galaxy A5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>2016 Galaxy A5</t>
@@ -356,95 +1444,222 @@
   </si>
   <si>
     <t>2016版 Galaxy A9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>2016 Galaxy A9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>麦芒3S</t>
-  </si>
-  <si>
-    <t>mmang 3s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>麦芒4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>mmang 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>麦芒3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>mmang 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>旗舰版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ultimate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>么么哒</t>
-  </si>
-  <si>
-    <t>s720t</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>么么哒3N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>星星1号</t>
-  </si>
-  <si>
-    <t>star1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>春雷HD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>7298d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>红牛V5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>redbull v5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TALK 7X八核</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>TALK 7X四核</t>
-  </si>
-  <si>
-    <t>talk 7x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>火星一号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>mars one</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>木星一号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>7295A青春版</t>
-  </si>
-  <si>
-    <t>7295a</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>大观4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>dag 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>小辣椒 M2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>chilli m2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>original model name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>new model name</t>
+    <t>小辣椒X4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小辣椒 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小辣椒5 Pro</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小辣椒 7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>红辣椒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>乐玩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>青春版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小苹果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>微客</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>天机3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>威武3C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金钢</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金刚II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雷霆战机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>旋影90w</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Razr V锋芒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>青漾3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>醉享</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Moto X极</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>魔镜 X5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小章鱼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T03锋至版</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>野火S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大Q Note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全魔王手机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>百利丰 W2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小黄蜂2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Z3D 梦想板</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ivvi 小i Plus</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -452,7 +1667,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,6 +1682,33 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Microsoft YaHei UI"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -809,10 +2051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A5546D8-4B7C-4F15-BF6A-F80DE1E85F51}">
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:B179"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -823,474 +2065,474 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>133</v>
+        <v>195</v>
       </c>
       <c r="B1" t="s">
-        <v>134</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.5">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>192</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>169</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>119</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>198</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>109</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>200</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>202</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>204</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>206</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>207</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>209</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>210</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>212</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>213</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>215</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>217</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>218</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>219</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>220</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>221</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>222</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>224</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>225</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>226</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>227</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>228</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>230</v>
       </c>
       <c r="B31" t="s">
-        <v>59</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>232</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>233</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>234</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>235</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B34" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>236</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>237</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>238</v>
       </c>
       <c r="B36" t="s">
-        <v>68</v>
+        <v>239</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>240</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>241</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>140</v>
       </c>
       <c r="B38" t="s">
-        <v>72</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B39" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>242</v>
       </c>
       <c r="B40" t="s">
-        <v>76</v>
+        <v>243</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>244</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>245</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>79</v>
+        <v>246</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>247</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>248</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>249</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>83</v>
+        <v>250</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
+        <v>251</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>85</v>
+        <v>252</v>
       </c>
       <c r="B45" t="s">
-        <v>86</v>
+        <v>253</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>254</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>255</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>90</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>91</v>
+        <v>256</v>
       </c>
       <c r="B48" t="s">
-        <v>92</v>
+        <v>257</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>93</v>
+        <v>258</v>
       </c>
       <c r="B49" t="s">
-        <v>94</v>
+        <v>259</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>95</v>
+        <v>260</v>
       </c>
       <c r="B50" t="s">
-        <v>96</v>
+        <v>261</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>42</v>
       </c>
       <c r="B51" t="s">
-        <v>98</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>99</v>
+        <v>262</v>
       </c>
       <c r="B52" t="s">
-        <v>100</v>
+        <v>263</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>101</v>
+        <v>264</v>
       </c>
       <c r="B53" t="s">
-        <v>102</v>
+        <v>237</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>103</v>
+        <v>189</v>
       </c>
       <c r="B54" t="s">
-        <v>104</v>
+        <v>190</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>105</v>
+        <v>265</v>
       </c>
       <c r="B55" t="s">
-        <v>106</v>
+        <v>266</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>107</v>
+        <v>267</v>
       </c>
       <c r="B56" t="s">
-        <v>108</v>
+        <v>268</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>109</v>
+        <v>269</v>
       </c>
       <c r="B57" t="s">
-        <v>110</v>
+        <v>270</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>111</v>
+        <v>271</v>
       </c>
       <c r="B58" t="s">
-        <v>112</v>
+        <v>272</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>113</v>
+        <v>273</v>
       </c>
       <c r="B59" t="s">
-        <v>114</v>
+        <v>274</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1303,66 +2545,954 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>117</v>
+        <v>275</v>
       </c>
       <c r="B61" t="s">
-        <v>118</v>
+        <v>276</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>119</v>
+        <v>277</v>
       </c>
       <c r="B62" t="s">
-        <v>120</v>
+        <v>278</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>121</v>
+        <v>59</v>
       </c>
       <c r="B63" t="s">
-        <v>122</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>123</v>
+        <v>10</v>
       </c>
       <c r="B64" t="s">
-        <v>124</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>125</v>
+        <v>279</v>
       </c>
       <c r="B65" t="s">
-        <v>126</v>
+        <v>280</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>127</v>
+        <v>161</v>
       </c>
       <c r="B66" t="s">
-        <v>128</v>
+        <v>162</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="B67" t="s">
-        <v>130</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
+        <v>163</v>
+      </c>
+      <c r="B68" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>135</v>
+      </c>
+      <c r="B69" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>281</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>27</v>
+      </c>
+      <c r="B71" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>179</v>
+      </c>
+      <c r="B72" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>171</v>
+      </c>
+      <c r="B73" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>282</v>
+      </c>
+      <c r="B75" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>284</v>
+      </c>
+      <c r="B76" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>117</v>
+      </c>
+      <c r="B77" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>286</v>
+      </c>
+      <c r="B78" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>287</v>
+      </c>
+      <c r="B79" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>289</v>
+      </c>
+      <c r="B80" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>291</v>
+      </c>
+      <c r="B81" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>123</v>
+      </c>
+      <c r="B82" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>101</v>
+      </c>
+      <c r="B83" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>99</v>
+      </c>
+      <c r="B84" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>293</v>
+      </c>
+      <c r="B85" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>73</v>
+      </c>
+      <c r="B86" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>295</v>
+      </c>
+      <c r="B87" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>297</v>
+      </c>
+      <c r="B88" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>299</v>
+      </c>
+      <c r="B89" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>53</v>
+      </c>
+      <c r="B90" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>159</v>
+      </c>
+      <c r="B91" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>301</v>
+      </c>
+      <c r="B92" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>67</v>
+      </c>
+      <c r="B93" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>69</v>
+      </c>
+      <c r="B94" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>95</v>
+      </c>
+      <c r="B95" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>30</v>
+      </c>
+      <c r="B96" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>303</v>
+      </c>
+      <c r="B97" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>304</v>
+      </c>
+      <c r="B98" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>306</v>
+      </c>
+      <c r="B99" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>308</v>
+      </c>
+      <c r="B100" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>310</v>
+      </c>
+      <c r="B101" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>93</v>
+      </c>
+      <c r="B102" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>311</v>
+      </c>
+      <c r="B103" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>312</v>
+      </c>
+      <c r="B104" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>37</v>
+      </c>
+      <c r="B105" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>313</v>
+      </c>
+      <c r="B106" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>315</v>
+      </c>
+      <c r="B107" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>317</v>
+      </c>
+      <c r="B108" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>318</v>
+      </c>
+      <c r="B109" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>136</v>
+      </c>
+      <c r="B110" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>319</v>
+      </c>
+      <c r="B111" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>321</v>
+      </c>
+      <c r="B112" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>151</v>
+      </c>
+      <c r="B113" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>322</v>
+      </c>
+      <c r="B114" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>105</v>
+      </c>
+      <c r="B115" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>323</v>
+      </c>
+      <c r="B116" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>146</v>
+      </c>
+      <c r="B117" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>325</v>
+      </c>
+      <c r="B118" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>50</v>
+      </c>
+      <c r="B119" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>127</v>
+      </c>
+      <c r="B120" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>111</v>
+      </c>
+      <c r="B121" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>327</v>
+      </c>
+      <c r="B122" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
+        <v>328</v>
+      </c>
+      <c r="B123" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
+        <v>97</v>
+      </c>
+      <c r="B124" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" t="s">
+        <v>186</v>
+      </c>
+      <c r="B125" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" t="s">
+        <v>329</v>
+      </c>
+      <c r="B126" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" t="s">
+        <v>107</v>
+      </c>
+      <c r="B127" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" t="s">
+        <v>330</v>
+      </c>
+      <c r="B128" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" ht="14.5">
+      <c r="A129" t="s">
+        <v>144</v>
+      </c>
+      <c r="B129" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" ht="14.5">
+      <c r="A130" t="s">
+        <v>154</v>
+      </c>
+      <c r="B130" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" ht="14.5">
+      <c r="A131" t="s">
+        <v>19</v>
+      </c>
+      <c r="B131" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" ht="14.5">
+      <c r="A132" t="s">
+        <v>61</v>
+      </c>
+      <c r="B132" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" ht="14.5">
+      <c r="A133" t="s">
+        <v>79</v>
+      </c>
+      <c r="B133" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="14.5">
+      <c r="A134" t="s">
+        <v>66</v>
+      </c>
+      <c r="B134" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" ht="14.5">
+      <c r="A135" t="s">
+        <v>149</v>
+      </c>
+      <c r="B135" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" t="s">
+        <v>331</v>
+      </c>
+      <c r="B136" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" t="s">
+        <v>20</v>
+      </c>
+      <c r="B137" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" t="s">
+        <v>22</v>
+      </c>
+      <c r="B138" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" t="s">
+        <v>29</v>
+      </c>
+      <c r="B139" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" t="s">
+        <v>31</v>
+      </c>
+      <c r="B140" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" t="s">
+        <v>35</v>
+      </c>
+      <c r="B141" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" t="s">
+        <v>138</v>
+      </c>
+      <c r="B142" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" t="s">
+        <v>36</v>
+      </c>
+      <c r="B143" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" t="s">
+        <v>167</v>
+      </c>
+      <c r="B144" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" t="s">
+        <v>165</v>
+      </c>
+      <c r="B145" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" t="s">
+        <v>332</v>
+      </c>
+      <c r="B146" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" t="s">
+        <v>48</v>
+      </c>
+      <c r="B147" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" t="s">
+        <v>333</v>
+      </c>
+      <c r="B148" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" t="s">
+        <v>87</v>
+      </c>
+      <c r="B149" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" t="s">
+        <v>51</v>
+      </c>
+      <c r="B150" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" t="s">
+        <v>56</v>
+      </c>
+      <c r="B151" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" t="s">
+        <v>57</v>
+      </c>
+      <c r="B152" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" t="s">
+        <v>334</v>
+      </c>
+      <c r="B153" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" t="s">
+        <v>335</v>
+      </c>
+      <c r="B154" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" t="s">
+        <v>336</v>
+      </c>
+      <c r="B155" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" ht="14.5">
+      <c r="A156" t="s">
+        <v>176</v>
+      </c>
+      <c r="B156" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" t="s">
+        <v>89</v>
+      </c>
+      <c r="B157" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" t="s">
+        <v>91</v>
+      </c>
+      <c r="B158" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" t="s">
+        <v>337</v>
+      </c>
+      <c r="B159" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" t="s">
+        <v>103</v>
+      </c>
+      <c r="B160" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" t="s">
+        <v>338</v>
+      </c>
+      <c r="B161" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162" t="s">
+        <v>339</v>
+      </c>
+      <c r="B162" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" t="s">
+        <v>340</v>
+      </c>
+      <c r="B163" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164" t="s">
+        <v>341</v>
+      </c>
+      <c r="B164" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165" t="s">
+        <v>342</v>
+      </c>
+      <c r="B165" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
+      <c r="A166" t="s">
+        <v>343</v>
+      </c>
+      <c r="B166" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167" t="s">
+        <v>130</v>
+      </c>
+      <c r="B167" t="s">
         <v>131</v>
       </c>
-      <c r="B68" t="s">
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168" t="s">
+        <v>344</v>
+      </c>
+      <c r="B168" t="s">
         <v>132</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="A169" t="s">
+        <v>345</v>
+      </c>
+      <c r="B169" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="A170" t="s">
+        <v>346</v>
+      </c>
+      <c r="B170" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="A171" t="s">
+        <v>347</v>
+      </c>
+      <c r="B171" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
+      <c r="A172" t="s">
+        <v>348</v>
+      </c>
+      <c r="B172" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
+      <c r="A173" t="s">
+        <v>349</v>
+      </c>
+      <c r="B173" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174" t="s">
+        <v>350</v>
+      </c>
+      <c r="B174" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
+      <c r="A175" t="s">
+        <v>351</v>
+      </c>
+      <c r="B175" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
+      <c r="A176" t="s">
+        <v>352</v>
+      </c>
+      <c r="B176" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177" t="s">
+        <v>353</v>
+      </c>
+      <c r="B177" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178" t="s">
+        <v>354</v>
+      </c>
+      <c r="B178" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179" t="s">
+        <v>355</v>
+      </c>
+      <c r="B179" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>